<commit_message>
add chinese name to moves
</commit_message>
<xml_diff>
--- a/charge_moves.xlsx
+++ b/charge_moves.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14580"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13520" windowHeight="14760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="305">
   <si>
     <t>bug</t>
   </si>
@@ -953,6 +953,486 @@
   </si>
   <si>
     <t>precipice blades</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>chName</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>超级角击</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>十字剪</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>信号光束</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>银色旋风</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>虫鸣</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>欺诈</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>恶之波动</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>暗袭要害</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>咬碎</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>龙之波动</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>逆鳞</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>龙爪</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>龙卷风</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>打雷</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>雷电拳</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>抛物面充电</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>疯狂伏特</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>放电</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>电磁炮</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>十万伏特</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>月亮之力</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>魔法闪耀</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>吸取之吻</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>嬉闹</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>魅惑之声</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>近身战</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>地狱翻滚</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>十字劈</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>真气弹</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>劈瓦</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>爆裂拳</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>蓄能焰袭</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>火焰拳</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>过热</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>火焰轮</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>喷射火焰</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>热风</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>勇鸟猛攻</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>燕返</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>暴风</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>影子偷袭</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>暗影球</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>日光束</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>蛮力藤鞭</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>能量球</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>叶刃</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>超级吸取</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>终极吸取</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>地震</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>极光束</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰冻光线</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰冻拳</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>雪崩</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰冻之风</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>暴风雪</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>破坏光线</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>挣扎</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>镜面反射</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>精神冲击</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>精神强念</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>岩崩</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>原始之力</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>尖石攻击</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>力量宝石</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁头</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>重磅冲撞</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>泡沫光线</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>水炮</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>水流喷射</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>水之波动</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>热水</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>断崖之剑</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>根源波动</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>冲浪</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>破灭之愿</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>流星群</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>陀螺球</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>加农光炮</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>磁铁炸弹</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>爱心印章</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>精神击破</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>预知未来</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>幻象光线</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>精神突进</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>盐水</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>泥巴炸弹</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>重踏</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>骨棒</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>流沙地狱</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>直冲钻</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>挖洞</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>打草结</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>落英缤纷</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>种子炸弹</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>大字爆炎</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>烈焰溅射</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>下盘踢</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>空气利刃</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>啄钻</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>神鸟猛攻</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑夜魔影</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>暗影拳</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>奇异之风</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>夹住</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>紧束</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>必杀门牙</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>高速星星</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>角撞</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>睡觉</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>泰山压顶</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>踩踏</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>剧毒牙</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>十字毒刃</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>污泥炸弹</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>污泥波</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>污泥攻击</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>垃圾射击</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>岩石爆击</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>岩石封锁</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -1383,7 +1863,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1391,10 +1871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G122"/>
+  <dimension ref="A1:H122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="A116" sqref="A116"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="H105" sqref="H105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1402,7 +1882,7 @@
     <col min="1" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14" thickBot="1">
+    <row r="1" spans="1:8" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -1424,8 +1904,11 @@
       <c r="G1" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="14" thickBot="1">
+      <c r="H1" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="14" thickBot="1">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -1447,8 +1930,11 @@
       <c r="G2" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="14" thickBot="1">
+      <c r="H2" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="14" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
@@ -1470,8 +1956,11 @@
       <c r="G3" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="27" thickBot="1">
+      <c r="H3" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="27" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>29</v>
       </c>
@@ -1493,8 +1982,11 @@
       <c r="G4" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="14" thickBot="1">
+      <c r="H4" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="14" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
@@ -1516,8 +2008,11 @@
       <c r="G5" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="14" thickBot="1">
+      <c r="H5" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="14" thickBot="1">
       <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
@@ -1539,8 +2034,11 @@
       <c r="G6" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="14" thickBot="1">
+      <c r="H6" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="14" thickBot="1">
       <c r="A7" s="3" t="s">
         <v>32</v>
       </c>
@@ -1562,8 +2060,11 @@
       <c r="G7" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="14" thickBot="1">
+      <c r="H7" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="14" thickBot="1">
       <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
@@ -1585,8 +2086,11 @@
       <c r="G8" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="14" thickBot="1">
+      <c r="H8" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="14" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>34</v>
       </c>
@@ -1608,8 +2112,11 @@
       <c r="G9" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="14" thickBot="1">
+      <c r="H9" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="14" thickBot="1">
       <c r="A10" s="3" t="s">
         <v>35</v>
       </c>
@@ -1631,8 +2138,11 @@
       <c r="G10" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="27" thickBot="1">
+      <c r="H10" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="27" thickBot="1">
       <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
@@ -1654,8 +2164,11 @@
       <c r="G11" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="14" thickBot="1">
+      <c r="H11" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="14" thickBot="1">
       <c r="A12" s="3" t="s">
         <v>37</v>
       </c>
@@ -1677,8 +2190,11 @@
       <c r="G12" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="27" thickBot="1">
+      <c r="H12" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="27" thickBot="1">
       <c r="A13" s="3" t="s">
         <v>38</v>
       </c>
@@ -1700,8 +2216,11 @@
       <c r="G13" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="14" thickBot="1">
+      <c r="H13" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="14" thickBot="1">
       <c r="A14" s="3" t="s">
         <v>39</v>
       </c>
@@ -1723,8 +2242,11 @@
       <c r="G14" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="14" thickBot="1">
+      <c r="H14" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="14" thickBot="1">
       <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
@@ -1746,8 +2268,11 @@
       <c r="G15" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="27" thickBot="1">
+      <c r="H15" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="27" thickBot="1">
       <c r="A16" s="3" t="s">
         <v>40</v>
       </c>
@@ -1769,8 +2294,11 @@
       <c r="G16" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="27" thickBot="1">
+      <c r="H16" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="27" thickBot="1">
       <c r="A17" s="3" t="s">
         <v>41</v>
       </c>
@@ -1792,8 +2320,11 @@
       <c r="G17" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="14" thickBot="1">
+      <c r="H17" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="14" thickBot="1">
       <c r="A18" s="3" t="s">
         <v>42</v>
       </c>
@@ -1815,8 +2346,11 @@
       <c r="G18" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="14" thickBot="1">
+      <c r="H18" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="14" thickBot="1">
       <c r="A19" s="3" t="s">
         <v>43</v>
       </c>
@@ -1838,8 +2372,11 @@
       <c r="G19" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="27" thickBot="1">
+      <c r="H19" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="27" thickBot="1">
       <c r="A20" s="3" t="s">
         <v>44</v>
       </c>
@@ -1861,8 +2398,11 @@
       <c r="G20" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="14" thickBot="1">
+      <c r="H20" s="4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="14" thickBot="1">
       <c r="A21" s="3" t="s">
         <v>45</v>
       </c>
@@ -1884,8 +2424,11 @@
       <c r="G21" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="14" thickBot="1">
+      <c r="H21" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="14" thickBot="1">
       <c r="A22" s="3" t="s">
         <v>46</v>
       </c>
@@ -1907,8 +2450,11 @@
       <c r="G22" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="27" thickBot="1">
+      <c r="H22" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="27" thickBot="1">
       <c r="A23" s="3" t="s">
         <v>47</v>
       </c>
@@ -1930,8 +2476,11 @@
       <c r="G23" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="27" thickBot="1">
+      <c r="H23" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="27" thickBot="1">
       <c r="A24" s="3" t="s">
         <v>48</v>
       </c>
@@ -1953,8 +2502,11 @@
       <c r="G24" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="14" thickBot="1">
+      <c r="H24" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="14" thickBot="1">
       <c r="A25" s="3" t="s">
         <v>49</v>
       </c>
@@ -1976,8 +2528,11 @@
       <c r="G25" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="27" thickBot="1">
+      <c r="H25" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="27" thickBot="1">
       <c r="A26" s="3" t="s">
         <v>50</v>
       </c>
@@ -1999,8 +2554,11 @@
       <c r="G26" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="27" thickBot="1">
+      <c r="H26" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="27" thickBot="1">
       <c r="A27" s="3" t="s">
         <v>51</v>
       </c>
@@ -2022,8 +2580,11 @@
       <c r="G27" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="14" thickBot="1">
+      <c r="H27" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="14" thickBot="1">
       <c r="A28" s="3" t="s">
         <v>52</v>
       </c>
@@ -2045,8 +2606,11 @@
       <c r="G28" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="14" thickBot="1">
+      <c r="H28" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="14" thickBot="1">
       <c r="A29" s="3" t="s">
         <v>53</v>
       </c>
@@ -2068,8 +2632,11 @@
       <c r="G29" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="14" thickBot="1">
+      <c r="H29" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="14" thickBot="1">
       <c r="A30" s="3" t="s">
         <v>54</v>
       </c>
@@ -2091,8 +2658,11 @@
       <c r="G30" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="14" thickBot="1">
+      <c r="H30" s="4" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="14" thickBot="1">
       <c r="A31" s="3" t="s">
         <v>55</v>
       </c>
@@ -2114,8 +2684,11 @@
       <c r="G31" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="14" thickBot="1">
+      <c r="H31" s="4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="14" thickBot="1">
       <c r="A32" s="3" t="s">
         <v>56</v>
       </c>
@@ -2137,8 +2710,11 @@
       <c r="G32" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="27" thickBot="1">
+      <c r="H32" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="27" thickBot="1">
       <c r="A33" s="3" t="s">
         <v>57</v>
       </c>
@@ -2160,8 +2736,11 @@
       <c r="G33" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="27" thickBot="1">
+      <c r="H33" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="27" thickBot="1">
       <c r="A34" s="3" t="s">
         <v>58</v>
       </c>
@@ -2183,8 +2762,11 @@
       <c r="G34" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="14" thickBot="1">
+      <c r="H34" s="4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="14" thickBot="1">
       <c r="A35" s="3" t="s">
         <v>59</v>
       </c>
@@ -2206,8 +2788,11 @@
       <c r="G35" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="14" thickBot="1">
+      <c r="H35" s="4" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="14" thickBot="1">
       <c r="A36" s="3" t="s">
         <v>60</v>
       </c>
@@ -2229,8 +2814,11 @@
       <c r="G36" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="14" thickBot="1">
+      <c r="H36" s="4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="14" thickBot="1">
       <c r="A37" s="3" t="s">
         <v>61</v>
       </c>
@@ -2252,8 +2840,11 @@
       <c r="G37" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="27" thickBot="1">
+      <c r="H37" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="27" thickBot="1">
       <c r="A38" s="3" t="s">
         <v>62</v>
       </c>
@@ -2275,8 +2866,11 @@
       <c r="G38" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="14" thickBot="1">
+      <c r="H38" s="4" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="14" thickBot="1">
       <c r="A39" s="3" t="s">
         <v>63</v>
       </c>
@@ -2298,8 +2892,11 @@
       <c r="G39" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="27" thickBot="1">
+      <c r="H39" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="27" thickBot="1">
       <c r="A40" s="3" t="s">
         <v>64</v>
       </c>
@@ -2321,8 +2918,11 @@
       <c r="G40" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="14" thickBot="1">
+      <c r="H40" s="4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="14" thickBot="1">
       <c r="A41" s="3" t="s">
         <v>65</v>
       </c>
@@ -2344,8 +2944,11 @@
       <c r="G41" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="14" thickBot="1">
+      <c r="H41" s="4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="14" thickBot="1">
       <c r="A42" s="3" t="s">
         <v>66</v>
       </c>
@@ -2367,8 +2970,11 @@
       <c r="G42" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="14" thickBot="1">
+      <c r="H42" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="14" thickBot="1">
       <c r="A43" s="3" t="s">
         <v>67</v>
       </c>
@@ -2390,8 +2996,11 @@
       <c r="G43" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="14" thickBot="1">
+      <c r="H43" s="4" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="14" thickBot="1">
       <c r="A44" s="3" t="s">
         <v>68</v>
       </c>
@@ -2413,8 +3022,11 @@
       <c r="G44" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="14" thickBot="1">
+      <c r="H44" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="14" thickBot="1">
       <c r="A45" s="3" t="s">
         <v>69</v>
       </c>
@@ -2436,8 +3048,11 @@
       <c r="G45" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" ht="14" thickBot="1">
+      <c r="H45" s="4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="14" thickBot="1">
       <c r="A46" s="3" t="s">
         <v>70</v>
       </c>
@@ -2459,8 +3074,11 @@
       <c r="G46" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" ht="14" thickBot="1">
+      <c r="H46" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="14" thickBot="1">
       <c r="A47" s="3" t="s">
         <v>71</v>
       </c>
@@ -2482,8 +3100,11 @@
       <c r="G47" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="27" thickBot="1">
+      <c r="H47" s="4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="27" thickBot="1">
       <c r="A48" s="3" t="s">
         <v>72</v>
       </c>
@@ -2505,8 +3126,11 @@
       <c r="G48" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" ht="27" thickBot="1">
+      <c r="H48" s="4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="27" thickBot="1">
       <c r="A49" s="3" t="s">
         <v>73</v>
       </c>
@@ -2528,8 +3152,11 @@
       <c r="G49" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" ht="27" thickBot="1">
+      <c r="H49" s="4" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="27" thickBot="1">
       <c r="A50" s="3" t="s">
         <v>74</v>
       </c>
@@ -2551,8 +3178,11 @@
       <c r="G50" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" ht="27" thickBot="1">
+      <c r="H50" s="4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="27" thickBot="1">
       <c r="A51" s="3" t="s">
         <v>75</v>
       </c>
@@ -2574,8 +3204,11 @@
       <c r="G51" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" ht="27" thickBot="1">
+      <c r="H51" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="27" thickBot="1">
       <c r="A52" s="3" t="s">
         <v>76</v>
       </c>
@@ -2597,8 +3230,11 @@
       <c r="G52" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" ht="14" thickBot="1">
+      <c r="H52" s="4" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="14" thickBot="1">
       <c r="A53" s="3" t="s">
         <v>77</v>
       </c>
@@ -2620,8 +3256,11 @@
       <c r="G53" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" ht="14" thickBot="1">
+      <c r="H53" s="4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="14" thickBot="1">
       <c r="A54" s="3" t="s">
         <v>78</v>
       </c>
@@ -2643,8 +3282,11 @@
       <c r="G54" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" ht="14" thickBot="1">
+      <c r="H54" s="4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="14" thickBot="1">
       <c r="A55" s="3" t="s">
         <v>79</v>
       </c>
@@ -2666,8 +3308,11 @@
       <c r="G55" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" ht="14" thickBot="1">
+      <c r="H55" s="4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="14" thickBot="1">
       <c r="A56" s="3" t="s">
         <v>80</v>
       </c>
@@ -2689,8 +3334,11 @@
       <c r="G56" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" ht="14" thickBot="1">
+      <c r="H56" s="4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="14" thickBot="1">
       <c r="A57" s="3" t="s">
         <v>81</v>
       </c>
@@ -2712,8 +3360,11 @@
       <c r="G57" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" ht="27" thickBot="1">
+      <c r="H57" s="4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="27" thickBot="1">
       <c r="A58" s="3" t="s">
         <v>82</v>
       </c>
@@ -2735,8 +3386,11 @@
       <c r="G58" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" ht="14" thickBot="1">
+      <c r="H58" s="4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="14" thickBot="1">
       <c r="A59" s="3" t="s">
         <v>83</v>
       </c>
@@ -2758,8 +3412,11 @@
       <c r="G59" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" ht="14" thickBot="1">
+      <c r="H59" s="4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="14" thickBot="1">
       <c r="A60" s="3" t="s">
         <v>84</v>
       </c>
@@ -2781,8 +3438,11 @@
       <c r="G60" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" ht="14" thickBot="1">
+      <c r="H60" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="14" thickBot="1">
       <c r="A61" s="3" t="s">
         <v>85</v>
       </c>
@@ -2804,8 +3464,11 @@
       <c r="G61" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" ht="14" thickBot="1">
+      <c r="H61" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="14" thickBot="1">
       <c r="A62" s="3" t="s">
         <v>86</v>
       </c>
@@ -2827,8 +3490,11 @@
       <c r="G62" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" ht="14" thickBot="1">
+      <c r="H62" s="4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="14" thickBot="1">
       <c r="A63" s="3" t="s">
         <v>87</v>
       </c>
@@ -2850,8 +3516,11 @@
       <c r="G63" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" ht="14" thickBot="1">
+      <c r="H63" s="4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="14" thickBot="1">
       <c r="A64" s="3" t="s">
         <v>88</v>
       </c>
@@ -2873,8 +3542,11 @@
       <c r="G64" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" ht="14" thickBot="1">
+      <c r="H64" s="4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="14" thickBot="1">
       <c r="A65" s="3" t="s">
         <v>89</v>
       </c>
@@ -2896,8 +3568,11 @@
       <c r="G65" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" ht="14" thickBot="1">
+      <c r="H65" s="4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="14" thickBot="1">
       <c r="A66" s="3" t="s">
         <v>90</v>
       </c>
@@ -2919,8 +3594,11 @@
       <c r="G66" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" ht="14" thickBot="1">
+      <c r="H66" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="14" thickBot="1">
       <c r="A67" s="3" t="s">
         <v>91</v>
       </c>
@@ -2942,8 +3620,11 @@
       <c r="G67" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" ht="14" thickBot="1">
+      <c r="H67" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="14" thickBot="1">
       <c r="A68" s="3" t="s">
         <v>92</v>
       </c>
@@ -2965,8 +3646,11 @@
       <c r="G68" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" ht="27" thickBot="1">
+      <c r="H68" s="4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="27" thickBot="1">
       <c r="A69" s="3" t="s">
         <v>93</v>
       </c>
@@ -2988,8 +3672,11 @@
       <c r="G69" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" ht="14" thickBot="1">
+      <c r="H69" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="14" thickBot="1">
       <c r="A70" s="3" t="s">
         <v>94</v>
       </c>
@@ -3011,8 +3698,11 @@
       <c r="G70" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" ht="14" thickBot="1">
+      <c r="H70" s="4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="14" thickBot="1">
       <c r="A71" s="3" t="s">
         <v>95</v>
       </c>
@@ -3034,8 +3724,11 @@
       <c r="G71" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" ht="14" thickBot="1">
+      <c r="H71" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="14" thickBot="1">
       <c r="A72" s="3" t="s">
         <v>96</v>
       </c>
@@ -3057,8 +3750,11 @@
       <c r="G72" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" ht="14" thickBot="1">
+      <c r="H72" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="14" thickBot="1">
       <c r="A73" s="3" t="s">
         <v>97</v>
       </c>
@@ -3080,8 +3776,11 @@
       <c r="G73" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" ht="14" thickBot="1">
+      <c r="H73" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="14" thickBot="1">
       <c r="A74" s="3" t="s">
         <v>98</v>
       </c>
@@ -3103,8 +3802,11 @@
       <c r="G74" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" ht="14" thickBot="1">
+      <c r="H74" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="14" thickBot="1">
       <c r="A75" s="3" t="s">
         <v>99</v>
       </c>
@@ -3126,8 +3828,11 @@
       <c r="G75" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" ht="27" thickBot="1">
+      <c r="H75" s="4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="27" thickBot="1">
       <c r="A76" s="3" t="s">
         <v>100</v>
       </c>
@@ -3149,8 +3854,11 @@
       <c r="G76" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" ht="14" thickBot="1">
+      <c r="H76" s="4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="14" thickBot="1">
       <c r="A77" s="3" t="s">
         <v>101</v>
       </c>
@@ -3172,8 +3880,11 @@
       <c r="G77" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" ht="14" thickBot="1">
+      <c r="H77" s="4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="14" thickBot="1">
       <c r="A78" s="3" t="s">
         <v>102</v>
       </c>
@@ -3195,8 +3906,11 @@
       <c r="G78" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" ht="14" thickBot="1">
+      <c r="H78" s="4" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="14" thickBot="1">
       <c r="A79" s="3" t="s">
         <v>103</v>
       </c>
@@ -3218,8 +3932,11 @@
       <c r="G79" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" ht="14" thickBot="1">
+      <c r="H79" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="14" thickBot="1">
       <c r="A80" s="3" t="s">
         <v>104</v>
       </c>
@@ -3241,8 +3958,11 @@
       <c r="G80" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" ht="14" thickBot="1">
+      <c r="H80" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="14" thickBot="1">
       <c r="A81" s="3" t="s">
         <v>105</v>
       </c>
@@ -3264,8 +3984,11 @@
       <c r="G81" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" ht="14" thickBot="1">
+      <c r="H81" s="4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="14" thickBot="1">
       <c r="A82" s="3" t="s">
         <v>106</v>
       </c>
@@ -3287,8 +4010,11 @@
       <c r="G82" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" ht="14" thickBot="1">
+      <c r="H82" s="4" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="14" thickBot="1">
       <c r="A83" s="3" t="s">
         <v>107</v>
       </c>
@@ -3310,8 +4036,11 @@
       <c r="G83" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" ht="14" thickBot="1">
+      <c r="H83" s="4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="14" thickBot="1">
       <c r="A84" s="3" t="s">
         <v>108</v>
       </c>
@@ -3333,8 +4062,11 @@
       <c r="G84" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" ht="27" thickBot="1">
+      <c r="H84" s="4" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="27" thickBot="1">
       <c r="A85" s="3" t="s">
         <v>109</v>
       </c>
@@ -3356,8 +4088,11 @@
       <c r="G85" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" ht="27" thickBot="1">
+      <c r="H85" s="4" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="27" thickBot="1">
       <c r="A86" s="3" t="s">
         <v>110</v>
       </c>
@@ -3379,8 +4114,11 @@
       <c r="G86" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" ht="27" thickBot="1">
+      <c r="H86" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="27" thickBot="1">
       <c r="A87" s="3" t="s">
         <v>111</v>
       </c>
@@ -3402,8 +4140,11 @@
       <c r="G87" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" ht="14" thickBot="1">
+      <c r="H87" s="4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="14" thickBot="1">
       <c r="A88" s="3" t="s">
         <v>112</v>
       </c>
@@ -3425,8 +4166,11 @@
       <c r="G88" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" ht="14" thickBot="1">
+      <c r="H88" s="4" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="14" thickBot="1">
       <c r="A89" s="3" t="s">
         <v>113</v>
       </c>
@@ -3448,8 +4192,11 @@
       <c r="G89" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" ht="27" thickBot="1">
+      <c r="H89" s="4" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="27" thickBot="1">
       <c r="A90" s="3" t="s">
         <v>114</v>
       </c>
@@ -3471,8 +4218,11 @@
       <c r="G90" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" ht="27" thickBot="1">
+      <c r="H90" s="4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="27" thickBot="1">
       <c r="A91" s="3" t="s">
         <v>115</v>
       </c>
@@ -3494,8 +4244,11 @@
       <c r="G91" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" ht="14" thickBot="1">
+      <c r="H91" s="4" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="14" thickBot="1">
       <c r="A92" s="3" t="s">
         <v>15</v>
       </c>
@@ -3517,8 +4270,11 @@
       <c r="G92" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" ht="14" thickBot="1">
+      <c r="H92" s="4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="14" thickBot="1">
       <c r="A93" s="3" t="s">
         <v>16</v>
       </c>
@@ -3540,8 +4296,11 @@
       <c r="G93" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" ht="14" thickBot="1">
+      <c r="H93" s="4" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="14" thickBot="1">
       <c r="A94" s="3" t="s">
         <v>116</v>
       </c>
@@ -3563,8 +4322,11 @@
       <c r="G94" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" ht="14" thickBot="1">
+      <c r="H94" s="4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="14" thickBot="1">
       <c r="A95" s="3" t="s">
         <v>117</v>
       </c>
@@ -3586,8 +4348,11 @@
       <c r="G95" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" ht="14" thickBot="1">
+      <c r="H95" s="4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="14" thickBot="1">
       <c r="A96" s="3" t="s">
         <v>118</v>
       </c>
@@ -3609,8 +4374,11 @@
       <c r="G96" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" ht="14" thickBot="1">
+      <c r="H96" s="4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="14" thickBot="1">
       <c r="A97" s="3" t="s">
         <v>17</v>
       </c>
@@ -3632,8 +4400,11 @@
       <c r="G97" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" ht="14" thickBot="1">
+      <c r="H97" s="4" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="14" thickBot="1">
       <c r="A98" s="3" t="s">
         <v>119</v>
       </c>
@@ -3655,8 +4426,11 @@
       <c r="G98" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" ht="14" thickBot="1">
+      <c r="H98" s="4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="14" thickBot="1">
       <c r="A99" s="3" t="s">
         <v>120</v>
       </c>
@@ -3678,8 +4452,11 @@
       <c r="G99" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" ht="27" thickBot="1">
+      <c r="H99" s="4" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="27" thickBot="1">
       <c r="A100" s="3" t="s">
         <v>121</v>
       </c>
@@ -3701,8 +4478,11 @@
       <c r="G100" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" ht="14" thickBot="1">
+      <c r="H100" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="14" thickBot="1">
       <c r="A101" s="3" t="s">
         <v>122</v>
       </c>
@@ -3724,8 +4504,11 @@
       <c r="G101" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" ht="14" thickBot="1">
+      <c r="H101" s="4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="14" thickBot="1">
       <c r="A102" s="3" t="s">
         <v>123</v>
       </c>
@@ -3747,8 +4530,11 @@
       <c r="G102" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" ht="14" thickBot="1">
+      <c r="H102" s="4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="14" thickBot="1">
       <c r="A103" s="3" t="s">
         <v>124</v>
       </c>
@@ -3770,8 +4556,11 @@
       <c r="G103" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" ht="27" thickBot="1">
+      <c r="H103" s="4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="27" thickBot="1">
       <c r="A104" s="3" t="s">
         <v>125</v>
       </c>
@@ -3793,8 +4582,11 @@
       <c r="G104" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" ht="14" thickBot="1">
+      <c r="H104" s="4" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="14" thickBot="1">
       <c r="A105" s="3" t="s">
         <v>126</v>
       </c>
@@ -3816,8 +4608,11 @@
       <c r="G105" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" ht="14" thickBot="1">
+      <c r="H105" s="4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="14" thickBot="1">
       <c r="A106" s="3" t="s">
         <v>127</v>
       </c>
@@ -3839,8 +4634,11 @@
       <c r="G106" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" ht="14" thickBot="1">
+      <c r="H106" s="4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="14" thickBot="1">
       <c r="A107" s="3" t="s">
         <v>128</v>
       </c>
@@ -3862,8 +4660,11 @@
       <c r="G107" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" ht="27" thickBot="1">
+      <c r="H107" s="4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="27" thickBot="1">
       <c r="A108" s="3" t="s">
         <v>129</v>
       </c>
@@ -3885,8 +4686,11 @@
       <c r="G108" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" ht="27" thickBot="1">
+      <c r="H108" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="27" thickBot="1">
       <c r="A109" s="3" t="s">
         <v>130</v>
       </c>
@@ -3908,8 +4712,11 @@
       <c r="G109" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" ht="27" thickBot="1">
+      <c r="H109" s="4" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="27" thickBot="1">
       <c r="A110" s="3" t="s">
         <v>131</v>
       </c>
@@ -3931,8 +4738,11 @@
       <c r="G110" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" ht="14" thickBot="1">
+      <c r="H110" s="4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="14" thickBot="1">
       <c r="A111" s="3" t="s">
         <v>132</v>
       </c>
@@ -3955,7 +4765,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="14" thickBot="1">
+    <row r="112" spans="1:8" ht="14" thickBot="1">
       <c r="A112" s="3" t="s">
         <v>133</v>
       </c>
@@ -3977,8 +4787,11 @@
       <c r="G112" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" ht="14" thickBot="1">
+      <c r="H112" s="4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="14" thickBot="1">
       <c r="A113" s="3" t="s">
         <v>134</v>
       </c>
@@ -4000,8 +4813,11 @@
       <c r="G113" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" ht="27" thickBot="1">
+      <c r="H113" s="4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="27" thickBot="1">
       <c r="A114" s="3" t="s">
         <v>135</v>
       </c>
@@ -4023,8 +4839,11 @@
       <c r="G114" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" ht="13">
+      <c r="H114" s="4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="13">
       <c r="A115" s="3" t="s">
         <v>136</v>
       </c>
@@ -4046,8 +4865,11 @@
       <c r="G115" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" ht="26">
+      <c r="H115" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="26">
       <c r="A116" s="5" t="s">
         <v>184</v>
       </c>
@@ -4069,8 +4891,11 @@
       <c r="G116" s="4" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" ht="13">
+      <c r="H116" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="13">
       <c r="A117" s="6" t="s">
         <v>181</v>
       </c>
@@ -4092,8 +4917,11 @@
       <c r="G117" s="4" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" ht="13">
+      <c r="H117" s="4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="13">
       <c r="A118" s="6" t="s">
         <v>182</v>
       </c>
@@ -4115,8 +4943,11 @@
       <c r="G118" s="4" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" ht="13">
+      <c r="H118" s="4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="13">
       <c r="A119" s="6" t="s">
         <v>183</v>
       </c>
@@ -4138,8 +4969,11 @@
       <c r="G119" s="4" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" ht="13">
+      <c r="H119" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="13">
       <c r="A120" s="6" t="s">
         <v>180</v>
       </c>
@@ -4161,8 +4995,11 @@
       <c r="G120" s="4" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" ht="13">
+      <c r="H120" s="4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="13">
       <c r="A121" s="6" t="s">
         <v>179</v>
       </c>
@@ -4184,8 +5021,11 @@
       <c r="G121" s="4" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" ht="13">
+      <c r="H121" s="4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="13">
       <c r="A122" s="6"/>
       <c r="B122" s="6"/>
       <c r="C122" s="6"/>

</xml_diff>

<commit_message>
add chinese name search for move search
</commit_message>
<xml_diff>
--- a/charge_moves.xlsx
+++ b/charge_moves.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13520" windowHeight="14760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="306">
   <si>
     <t>bug</t>
   </si>
@@ -1433,6 +1433,10 @@
   </si>
   <si>
     <t>岩石封锁</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>水流尾</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -1863,7 +1867,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1873,8 +1877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="H105" sqref="H105"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="I112" sqref="I112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -4763,6 +4767,9 @@
       </c>
       <c r="G111" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="H111" s="4" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="14" thickBot="1">

</xml_diff>

<commit_message>
power whip ch name
</commit_message>
<xml_diff>
--- a/charge_moves.xlsx
+++ b/charge_moves.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -1132,10 +1132,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>蛮力藤鞭</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>能量球</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -1437,6 +1433,10 @@
   </si>
   <si>
     <t>水流尾</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>强力鞭打</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -1867,7 +1867,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1877,8 +1877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="I112" sqref="I112"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2663,7 +2663,7 @@
         <v>6</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="14" thickBot="1">
@@ -2819,7 +2819,7 @@
         <v>7</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="14" thickBot="1">
@@ -2897,7 +2897,7 @@
         <v>7</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="27" thickBot="1">
@@ -3001,7 +3001,7 @@
         <v>8</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="14" thickBot="1">
@@ -3079,7 +3079,7 @@
         <v>8</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="14" thickBot="1">
@@ -3105,7 +3105,7 @@
         <v>8</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="27" thickBot="1">
@@ -3131,7 +3131,7 @@
         <v>9</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="27" thickBot="1">
@@ -3157,7 +3157,7 @@
         <v>9</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="27" thickBot="1">
@@ -3235,7 +3235,7 @@
         <v>9</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="14" thickBot="1">
@@ -3261,7 +3261,7 @@
         <v>10</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="14" thickBot="1">
@@ -3287,7 +3287,7 @@
         <v>10</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="14" thickBot="1">
@@ -3339,7 +3339,7 @@
         <v>10</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="14" thickBot="1">
@@ -3365,7 +3365,7 @@
         <v>10</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>229</v>
+        <v>305</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="27" thickBot="1">
@@ -3391,7 +3391,7 @@
         <v>10</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="14" thickBot="1">
@@ -3417,7 +3417,7 @@
         <v>10</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="14" thickBot="1">
@@ -3443,7 +3443,7 @@
         <v>10</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="14" thickBot="1">
@@ -3469,7 +3469,7 @@
         <v>10</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="14" thickBot="1">
@@ -3495,7 +3495,7 @@
         <v>11</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="14" thickBot="1">
@@ -3521,7 +3521,7 @@
         <v>11</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="14" thickBot="1">
@@ -3547,7 +3547,7 @@
         <v>11</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="14" thickBot="1">
@@ -3573,7 +3573,7 @@
         <v>11</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="14" thickBot="1">
@@ -3599,7 +3599,7 @@
         <v>11</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="14" thickBot="1">
@@ -3625,7 +3625,7 @@
         <v>11</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="14" thickBot="1">
@@ -3651,7 +3651,7 @@
         <v>11</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="27" thickBot="1">
@@ -3677,7 +3677,7 @@
         <v>12</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="14" thickBot="1">
@@ -3703,7 +3703,7 @@
         <v>12</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="14" thickBot="1">
@@ -3729,7 +3729,7 @@
         <v>12</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="14" thickBot="1">
@@ -3755,7 +3755,7 @@
         <v>12</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="14" thickBot="1">
@@ -3781,7 +3781,7 @@
         <v>12</v>
       </c>
       <c r="H73" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="14" thickBot="1">
@@ -3807,7 +3807,7 @@
         <v>12</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="14" thickBot="1">
@@ -3833,7 +3833,7 @@
         <v>13</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="27" thickBot="1">
@@ -3859,7 +3859,7 @@
         <v>13</v>
       </c>
       <c r="H76" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="14" thickBot="1">
@@ -3885,7 +3885,7 @@
         <v>13</v>
       </c>
       <c r="H77" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="14" thickBot="1">
@@ -3911,7 +3911,7 @@
         <v>13</v>
       </c>
       <c r="H78" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="14" thickBot="1">
@@ -3937,7 +3937,7 @@
         <v>13</v>
       </c>
       <c r="H79" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="14" thickBot="1">
@@ -3963,7 +3963,7 @@
         <v>13</v>
       </c>
       <c r="H80" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="14" thickBot="1">
@@ -3989,7 +3989,7 @@
         <v>13</v>
       </c>
       <c r="H81" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="14" thickBot="1">
@@ -4015,7 +4015,7 @@
         <v>13</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="14" thickBot="1">
@@ -4041,7 +4041,7 @@
         <v>13</v>
       </c>
       <c r="H83" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="14" thickBot="1">
@@ -4067,7 +4067,7 @@
         <v>13</v>
       </c>
       <c r="H84" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="27" thickBot="1">
@@ -4093,7 +4093,7 @@
         <v>14</v>
       </c>
       <c r="H85" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="27" thickBot="1">
@@ -4119,7 +4119,7 @@
         <v>14</v>
       </c>
       <c r="H86" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="27" thickBot="1">
@@ -4145,7 +4145,7 @@
         <v>14</v>
       </c>
       <c r="H87" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="14" thickBot="1">
@@ -4171,7 +4171,7 @@
         <v>14</v>
       </c>
       <c r="H88" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="14" thickBot="1">
@@ -4197,7 +4197,7 @@
         <v>14</v>
       </c>
       <c r="H89" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="27" thickBot="1">
@@ -4223,7 +4223,7 @@
         <v>14</v>
       </c>
       <c r="H90" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="27" thickBot="1">
@@ -4249,7 +4249,7 @@
         <v>17</v>
       </c>
       <c r="H91" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="14" thickBot="1">
@@ -4275,7 +4275,7 @@
         <v>17</v>
       </c>
       <c r="H92" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="14" thickBot="1">
@@ -4301,7 +4301,7 @@
         <v>17</v>
       </c>
       <c r="H93" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="14" thickBot="1">
@@ -4327,7 +4327,7 @@
         <v>17</v>
       </c>
       <c r="H94" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="14" thickBot="1">
@@ -4353,7 +4353,7 @@
         <v>17</v>
       </c>
       <c r="H95" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="14" thickBot="1">
@@ -4379,7 +4379,7 @@
         <v>17</v>
       </c>
       <c r="H96" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="14" thickBot="1">
@@ -4405,7 +4405,7 @@
         <v>17</v>
       </c>
       <c r="H97" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="14" thickBot="1">
@@ -4431,7 +4431,7 @@
         <v>18</v>
       </c>
       <c r="H98" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="14" thickBot="1">
@@ -4457,7 +4457,7 @@
         <v>18</v>
       </c>
       <c r="H99" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="27" thickBot="1">
@@ -4483,7 +4483,7 @@
         <v>18</v>
       </c>
       <c r="H100" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="14" thickBot="1">
@@ -4509,7 +4509,7 @@
         <v>18</v>
       </c>
       <c r="H101" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="14" thickBot="1">
@@ -4535,7 +4535,7 @@
         <v>18</v>
       </c>
       <c r="H102" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="14" thickBot="1">
@@ -4561,7 +4561,7 @@
         <v>18</v>
       </c>
       <c r="H103" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="27" thickBot="1">
@@ -4587,7 +4587,7 @@
         <v>19</v>
       </c>
       <c r="H104" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="14" thickBot="1">
@@ -4613,7 +4613,7 @@
         <v>19</v>
       </c>
       <c r="H105" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="14" thickBot="1">
@@ -4639,7 +4639,7 @@
         <v>19</v>
       </c>
       <c r="H106" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="14" thickBot="1">
@@ -4665,7 +4665,7 @@
         <v>19</v>
       </c>
       <c r="H107" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="27" thickBot="1">
@@ -4691,7 +4691,7 @@
         <v>19</v>
       </c>
       <c r="H108" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="27" thickBot="1">
@@ -4717,7 +4717,7 @@
         <v>20</v>
       </c>
       <c r="H109" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="27" thickBot="1">
@@ -4743,7 +4743,7 @@
         <v>20</v>
       </c>
       <c r="H110" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="14" thickBot="1">
@@ -4769,7 +4769,7 @@
         <v>20</v>
       </c>
       <c r="H111" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="14" thickBot="1">
@@ -4795,7 +4795,7 @@
         <v>20</v>
       </c>
       <c r="H112" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="113" spans="1:8" ht="14" thickBot="1">
@@ -4821,7 +4821,7 @@
         <v>20</v>
       </c>
       <c r="H113" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="27" thickBot="1">
@@ -4847,7 +4847,7 @@
         <v>20</v>
       </c>
       <c r="H114" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="115" spans="1:8" ht="13">
@@ -4873,7 +4873,7 @@
         <v>20</v>
       </c>
       <c r="H115" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="26">
@@ -4899,7 +4899,7 @@
         <v>169</v>
       </c>
       <c r="H116" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="117" spans="1:8" ht="13">
@@ -4925,7 +4925,7 @@
         <v>171</v>
       </c>
       <c r="H117" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="13">
@@ -4951,7 +4951,7 @@
         <v>172</v>
       </c>
       <c r="H118" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="119" spans="1:8" ht="13">
@@ -4977,7 +4977,7 @@
         <v>177</v>
       </c>
       <c r="H119" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="120" spans="1:8" ht="13">
@@ -5003,7 +5003,7 @@
         <v>170</v>
       </c>
       <c r="H120" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="121" spans="1:8" ht="13">
@@ -5029,7 +5029,7 @@
         <v>170</v>
       </c>
       <c r="H121" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="13">

</xml_diff>

<commit_message>
round error + pgm update
</commit_message>
<xml_diff>
--- a/charge_moves.xlsx
+++ b/charge_moves.xlsx
@@ -1867,7 +1867,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1877,8 +1877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H57" sqref="H57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
format change+legacy move update
</commit_message>
<xml_diff>
--- a/charge_moves.xlsx
+++ b/charge_moves.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="321">
   <si>
     <t>bug</t>
   </si>
@@ -1472,6 +1472,34 @@
   </si>
   <si>
     <t>爆炸烈焰</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>last resort</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.9s</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>normal</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>珍藏</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>hydro cannon</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.9s</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>加农水炮</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -1569,8 +1597,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1610,7 +1640,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="25">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
@@ -1623,6 +1653,7 @@
     <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -1634,6 +1665,7 @@
     <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1911,10 +1943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H123"/>
+  <dimension ref="A1:H125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="H125" sqref="H125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2312,7 +2344,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="27" thickBot="1">
+    <row r="16" spans="1:8" ht="14" thickBot="1">
       <c r="A16" s="3" t="s">
         <v>3</v>
       </c>
@@ -2364,7 +2396,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="14" thickBot="1">
+    <row r="18" spans="1:8" ht="27" thickBot="1">
       <c r="A18" s="3" t="s">
         <v>41</v>
       </c>
@@ -2416,7 +2448,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="27" thickBot="1">
+    <row r="20" spans="1:8" ht="14" thickBot="1">
       <c r="A20" s="3" t="s">
         <v>43</v>
       </c>
@@ -2442,7 +2474,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="14" thickBot="1">
+    <row r="21" spans="1:8" ht="27" thickBot="1">
       <c r="A21" s="3" t="s">
         <v>44</v>
       </c>
@@ -2494,7 +2526,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="27" thickBot="1">
+    <row r="23" spans="1:8" ht="14" thickBot="1">
       <c r="A23" s="3" t="s">
         <v>46</v>
       </c>
@@ -2546,7 +2578,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="14" thickBot="1">
+    <row r="25" spans="1:8" ht="27" thickBot="1">
       <c r="A25" s="3" t="s">
         <v>48</v>
       </c>
@@ -2572,7 +2604,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="27" thickBot="1">
+    <row r="26" spans="1:8" ht="14" thickBot="1">
       <c r="A26" s="3" t="s">
         <v>49</v>
       </c>
@@ -2624,7 +2656,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="14" thickBot="1">
+    <row r="28" spans="1:8" ht="27" thickBot="1">
       <c r="A28" s="3" t="s">
         <v>51</v>
       </c>
@@ -2754,7 +2786,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="27" thickBot="1">
+    <row r="33" spans="1:8" ht="14" thickBot="1">
       <c r="A33" s="3" t="s">
         <v>56</v>
       </c>
@@ -2806,7 +2838,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="14" thickBot="1">
+    <row r="35" spans="1:8" ht="27" thickBot="1">
       <c r="A35" s="3" t="s">
         <v>58</v>
       </c>
@@ -2884,7 +2916,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="27" thickBot="1">
+    <row r="38" spans="1:8" ht="14" thickBot="1">
       <c r="A38" s="3" t="s">
         <v>61</v>
       </c>
@@ -2910,7 +2942,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="14" thickBot="1">
+    <row r="39" spans="1:8" ht="27" thickBot="1">
       <c r="A39" s="3" t="s">
         <v>62</v>
       </c>
@@ -2936,7 +2968,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="27" thickBot="1">
+    <row r="40" spans="1:8" ht="14" thickBot="1">
       <c r="A40" s="3" t="s">
         <v>63</v>
       </c>
@@ -2962,7 +2994,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="14" thickBot="1">
+    <row r="41" spans="1:8" ht="27" thickBot="1">
       <c r="A41" s="3" t="s">
         <v>64</v>
       </c>
@@ -3144,7 +3176,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="27" thickBot="1">
+    <row r="48" spans="1:8" ht="14" thickBot="1">
       <c r="A48" s="3" t="s">
         <v>70</v>
       </c>
@@ -3170,7 +3202,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="27" thickBot="1">
+    <row r="49" spans="1:8" ht="14" thickBot="1">
       <c r="A49" s="3" t="s">
         <v>71</v>
       </c>
@@ -3274,7 +3306,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="14" thickBot="1">
+    <row r="53" spans="1:8" ht="27" thickBot="1">
       <c r="A53" s="3" t="s">
         <v>75</v>
       </c>
@@ -3300,7 +3332,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="14" thickBot="1">
+    <row r="54" spans="1:8" ht="27" thickBot="1">
       <c r="A54" s="3" t="s">
         <v>76</v>
       </c>
@@ -3404,7 +3436,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="27" thickBot="1">
+    <row r="58" spans="1:8" ht="14" thickBot="1">
       <c r="A58" s="3" t="s">
         <v>80</v>
       </c>
@@ -3456,7 +3488,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="14" thickBot="1">
+    <row r="60" spans="1:8" ht="27" thickBot="1">
       <c r="A60" s="3" t="s">
         <v>82</v>
       </c>
@@ -3690,7 +3722,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="27" thickBot="1">
+    <row r="69" spans="1:8" ht="14" thickBot="1">
       <c r="A69" s="3" t="s">
         <v>90</v>
       </c>
@@ -3768,7 +3800,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="14" thickBot="1">
+    <row r="72" spans="1:8" ht="27" thickBot="1">
       <c r="A72" s="3" t="s">
         <v>184</v>
       </c>
@@ -3794,7 +3826,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="14" thickBot="1">
+    <row r="73" spans="1:8" ht="27" thickBot="1">
       <c r="A73" s="3" t="s">
         <v>93</v>
       </c>
@@ -3872,7 +3904,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="27" thickBot="1">
+    <row r="76" spans="1:8" ht="14" thickBot="1">
       <c r="A76" s="3" t="s">
         <v>96</v>
       </c>
@@ -3976,7 +4008,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="14" thickBot="1">
+    <row r="80" spans="1:8" ht="27" thickBot="1">
       <c r="A80" s="3" t="s">
         <v>100</v>
       </c>
@@ -4106,7 +4138,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="27" thickBot="1">
+    <row r="85" spans="1:8" ht="14" thickBot="1">
       <c r="A85" s="3" t="s">
         <v>105</v>
       </c>
@@ -4132,7 +4164,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="27" thickBot="1">
+    <row r="86" spans="1:8" ht="14" thickBot="1">
       <c r="A86" s="3" t="s">
         <v>106</v>
       </c>
@@ -4158,7 +4190,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="27" thickBot="1">
+    <row r="87" spans="1:8" ht="14" thickBot="1">
       <c r="A87" s="3" t="s">
         <v>107</v>
       </c>
@@ -4210,7 +4242,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="14" thickBot="1">
+    <row r="89" spans="1:8" ht="27" thickBot="1">
       <c r="A89" s="3" t="s">
         <v>109</v>
       </c>
@@ -4340,7 +4372,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="14" thickBot="1">
+    <row r="94" spans="1:8" ht="27" thickBot="1">
       <c r="A94" s="3" t="s">
         <v>114</v>
       </c>
@@ -4366,7 +4398,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="14" thickBot="1">
+    <row r="95" spans="1:8" ht="27" thickBot="1">
       <c r="A95" s="3" t="s">
         <v>115</v>
       </c>
@@ -4496,7 +4528,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="27" thickBot="1">
+    <row r="100" spans="1:8" ht="14" thickBot="1">
       <c r="A100" s="3" t="s">
         <v>118</v>
       </c>
@@ -4600,7 +4632,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="27" thickBot="1">
+    <row r="104" spans="1:8" ht="14" thickBot="1">
       <c r="A104" s="3" t="s">
         <v>120</v>
       </c>
@@ -4626,7 +4658,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="14" thickBot="1">
+    <row r="105" spans="1:8" ht="27" thickBot="1">
       <c r="A105" s="3" t="s">
         <v>121</v>
       </c>
@@ -4704,7 +4736,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="27" thickBot="1">
+    <row r="108" spans="1:8" ht="14" thickBot="1">
       <c r="A108" s="3" t="s">
         <v>124</v>
       </c>
@@ -4756,7 +4788,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="27" thickBot="1">
+    <row r="110" spans="1:8" ht="14" thickBot="1">
       <c r="A110" s="3" t="s">
         <v>126</v>
       </c>
@@ -4834,7 +4866,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="14" thickBot="1">
+    <row r="113" spans="1:8" ht="27" thickBot="1">
       <c r="A113" s="3" t="s">
         <v>129</v>
       </c>
@@ -4860,7 +4892,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="27" thickBot="1">
+    <row r="114" spans="1:8" ht="14" thickBot="1">
       <c r="A114" s="7" t="s">
         <v>181</v>
       </c>
@@ -4886,7 +4918,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="13">
+    <row r="115" spans="1:8" ht="26">
       <c r="A115" s="3" t="s">
         <v>130</v>
       </c>
@@ -5016,7 +5048,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="13">
+    <row r="120" spans="1:8" ht="26">
       <c r="A120" s="5" t="s">
         <v>135</v>
       </c>
@@ -5118,6 +5150,58 @@
       </c>
       <c r="H123" s="4" t="s">
         <v>258</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="13">
+      <c r="A124" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="B124" s="6">
+        <v>31</v>
+      </c>
+      <c r="C124" s="6">
+        <v>1.8</v>
+      </c>
+      <c r="D124" s="6">
+        <v>90</v>
+      </c>
+      <c r="E124" s="6">
+        <v>-50</v>
+      </c>
+      <c r="F124" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="G124" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="H124" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" ht="13">
+      <c r="A125" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="B125" s="6">
+        <v>47.4</v>
+      </c>
+      <c r="C125" s="6">
+        <v>1.8</v>
+      </c>
+      <c r="D125" s="6">
+        <v>90</v>
+      </c>
+      <c r="E125" s="6">
+        <v>-50</v>
+      </c>
+      <c r="F125" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="G125" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="H125" s="4" t="s">
+        <v>320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gen 4 move added
</commit_message>
<xml_diff>
--- a/charge_moves.xlsx
+++ b/charge_moves.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720"/>
+    <workbookView xWindow="15200" yWindow="760" windowWidth="25600" windowHeight="14720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="325">
   <si>
     <t>bug</t>
   </si>
@@ -1500,6 +1500,22 @@
   </si>
   <si>
     <t>加农水炮</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>meteor mash</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.6s</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>steel</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>彗星拳</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -1935,7 +1951,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1943,10 +1959,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H125"/>
+  <dimension ref="A1:H126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="H125" sqref="H125"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="C126" sqref="C126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -5202,6 +5218,32 @@
       </c>
       <c r="H125" s="4" t="s">
         <v>320</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="13">
+      <c r="A126" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="B126" s="6">
+        <v>38.5</v>
+      </c>
+      <c r="C126" s="6">
+        <v>2</v>
+      </c>
+      <c r="D126" s="6">
+        <v>100</v>
+      </c>
+      <c r="E126" s="6">
+        <v>-50</v>
+      </c>
+      <c r="F126" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="G126" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="H126" s="4" t="s">
+        <v>324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>